<commit_message>
data and report cleanup
</commit_message>
<xml_diff>
--- a/SensitivityAnalisys/CF_G_2023_1.xlsx
+++ b/SensitivityAnalisys/CF_G_2023_1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774DAD23-BE2A-492C-8FEA-321AEA91BCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B581753-31F6-4F42-9A7A-CDC7F191D5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52305" yWindow="5430" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
   <si>
     <t>ReportingNode</t>
   </si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>EV</t>
   </si>
 </sst>
 </file>
@@ -1111,75 +1120,75 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_Cashflow" displayName="Table_Cashflow" ref="A1:BN4" totalsRowShown="0">
-  <autoFilter ref="A1:BN4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{468DBC3D-0A65-4F14-9B32-8928DD0B1B61}" name="Table_Cashflow" displayName="Table_Cashflow" ref="A1:BN9" totalsRowShown="0">
+  <autoFilter ref="A1:BN9" xr:uid="{468DBC3D-0A65-4F14-9B32-8928DD0B1B61}"/>
   <tableColumns count="66">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DataNode" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="AmountType" dataDxfId="63"/>
-    <tableColumn id="66" xr3:uid="{FF1D6B8E-4B53-41CC-AEA1-72F0B116C742}" name="EstimateType"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="AocType" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Novelty" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Values0" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Values1" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Values2" dataDxfId="58"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Values3" dataDxfId="57"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Values4" dataDxfId="56"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Values5" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Values6" dataDxfId="54"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Values7" dataDxfId="53"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Values8" dataDxfId="52"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Values9" dataDxfId="51"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Values10" dataDxfId="50"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Values11" dataDxfId="49"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Values12" dataDxfId="48"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Values13" dataDxfId="47"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Values14" dataDxfId="46"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Values15" dataDxfId="45"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Values16" dataDxfId="44"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="Values17" dataDxfId="43"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Values18" dataDxfId="42"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Values19" dataDxfId="41"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="Values20" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{A29DD33B-AA8E-47A9-AA4B-B71FCA1EAF4A}" name="Values21" dataDxfId="39"/>
-    <tableColumn id="27" xr3:uid="{27224793-D751-44F0-925E-8C09A1B6EB74}" name="Values22" dataDxfId="38"/>
-    <tableColumn id="28" xr3:uid="{3CD31C34-CCC3-40EE-984D-B93AD1DB0033}" name="Values23" dataDxfId="37"/>
-    <tableColumn id="29" xr3:uid="{9A0AF289-0C6D-40B0-BB96-9918911C4BC8}" name="Values24" dataDxfId="36"/>
-    <tableColumn id="30" xr3:uid="{3BCC908C-AF0D-4CD0-BD94-76CB13313CBB}" name="Values25" dataDxfId="35"/>
-    <tableColumn id="31" xr3:uid="{45537A01-6098-467A-A6C7-99908C56F6F4}" name="Values26" dataDxfId="34"/>
-    <tableColumn id="32" xr3:uid="{6DA0E2ED-6650-4F95-896E-AC4531318194}" name="Values27" dataDxfId="33"/>
-    <tableColumn id="33" xr3:uid="{C000D778-9DE1-4A34-BAAD-AB8D3647DA05}" name="Values28" dataDxfId="32"/>
-    <tableColumn id="34" xr3:uid="{9DB029E7-572A-4742-BA58-9322EF256D67}" name="Values29" dataDxfId="31"/>
-    <tableColumn id="35" xr3:uid="{D556C89A-E63C-4A1B-87DE-8492C257AECA}" name="Values30" dataDxfId="30"/>
-    <tableColumn id="36" xr3:uid="{994F282E-8D18-40F6-A300-9603F37C9B4B}" name="Values31" dataDxfId="29"/>
-    <tableColumn id="37" xr3:uid="{CD479843-E653-41A0-AAF3-8AD090F21296}" name="Values32" dataDxfId="28"/>
-    <tableColumn id="38" xr3:uid="{8572D1A9-1FCD-4E7D-9C58-98F05BD952B0}" name="Values33" dataDxfId="27"/>
-    <tableColumn id="39" xr3:uid="{49E8BC14-3177-4C36-B225-58AC0D07092A}" name="Values34" dataDxfId="26"/>
-    <tableColumn id="40" xr3:uid="{C1E5D7EB-AA3A-4A18-A924-2C12A8B36766}" name="Values35" dataDxfId="25"/>
-    <tableColumn id="41" xr3:uid="{16C5A89E-FAAC-4516-9172-D72810A63D6B}" name="Values36" dataDxfId="24"/>
-    <tableColumn id="42" xr3:uid="{79F7250E-B111-4D95-80FF-5357712E2614}" name="Values37" dataDxfId="23"/>
-    <tableColumn id="43" xr3:uid="{2436675F-4429-41A6-A206-4AC7BD75E6F7}" name="Values38" dataDxfId="22"/>
-    <tableColumn id="44" xr3:uid="{16DEBACA-AA3A-476F-B015-E15CF87E6814}" name="Values39" dataDxfId="21"/>
-    <tableColumn id="45" xr3:uid="{CCCEE462-DBAA-4462-8918-963C628D6B20}" name="Values40" dataDxfId="20"/>
-    <tableColumn id="46" xr3:uid="{77B24BE9-A951-4AE9-A8B7-5C9214C3BCDD}" name="Values41" dataDxfId="19"/>
-    <tableColumn id="47" xr3:uid="{CD1EF11F-617A-41C3-9656-646B7182839B}" name="Values42" dataDxfId="18"/>
-    <tableColumn id="48" xr3:uid="{C73D090B-0498-4537-92D9-81BB5B4CC34C}" name="Values43" dataDxfId="17"/>
-    <tableColumn id="49" xr3:uid="{8EF45FE8-50FE-4228-A3B9-67902151D68F}" name="Values44" dataDxfId="16"/>
-    <tableColumn id="50" xr3:uid="{B251F40C-E01D-4E97-B6CE-63AA496491FC}" name="Values45" dataDxfId="15"/>
-    <tableColumn id="51" xr3:uid="{5842F1FA-8DC0-4ECC-B9B1-E74E8EC3295B}" name="Values46" dataDxfId="14"/>
-    <tableColumn id="52" xr3:uid="{C42A9FD3-A13C-4A9B-8A6D-DFA6040BE64B}" name="Values47" dataDxfId="13"/>
-    <tableColumn id="53" xr3:uid="{9BDF4A95-5490-4FD0-8BD4-33FBA0E5787D}" name="Values48" dataDxfId="12"/>
-    <tableColumn id="54" xr3:uid="{4F2F13ED-97F9-4BD0-8C9C-BBB360A3FD9C}" name="Values49" dataDxfId="11"/>
-    <tableColumn id="55" xr3:uid="{3406BB6C-5A6F-4014-94C3-858037D4ACB2}" name="Values50" dataDxfId="10"/>
-    <tableColumn id="56" xr3:uid="{7971DC9B-B3C3-4009-B8A6-7D594260EE1D}" name="Values51" dataDxfId="9"/>
-    <tableColumn id="57" xr3:uid="{3102D966-6D8F-4FB3-9947-88CE7FAD6457}" name="Values52" dataDxfId="8"/>
-    <tableColumn id="58" xr3:uid="{76AECBE0-E8A4-4272-8320-828175A01745}" name="Values53" dataDxfId="7"/>
-    <tableColumn id="59" xr3:uid="{EA7207F1-7B9D-4C0C-A643-A9C0F7819969}" name="Values54" dataDxfId="6"/>
-    <tableColumn id="60" xr3:uid="{5721B0B3-677D-4B0E-91E3-4318CEDA73A6}" name="Values55" dataDxfId="5"/>
-    <tableColumn id="61" xr3:uid="{F238A67D-A5C3-477C-B5C3-796F717011ED}" name="Values56" dataDxfId="4"/>
-    <tableColumn id="62" xr3:uid="{988BF362-C460-4FC5-9B09-36388DBC9163}" name="Values57" dataDxfId="3"/>
-    <tableColumn id="63" xr3:uid="{803A8654-2111-47AC-B5B4-D2E092402C7F}" name="Values58" dataDxfId="2"/>
-    <tableColumn id="64" xr3:uid="{E5DA66EA-7F0F-4E6F-946F-48688A21D3A8}" name="Values59" dataDxfId="1"/>
-    <tableColumn id="65" xr3:uid="{1876E55A-3F43-4C92-BE12-BCC76DBDABDD}" name="Values60" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{057B0D49-A8BD-499B-B2E4-E195B841EFC6}" name="DataNode" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{509FE89C-4F86-467C-A8A2-DD4211DAD010}" name="AmountType" dataDxfId="63"/>
+    <tableColumn id="66" xr3:uid="{32355EEA-C273-483A-AA9D-EAA4EF397828}" name="EstimateType"/>
+    <tableColumn id="3" xr3:uid="{5FDD8AC2-4628-4EB6-BBC2-42EB6858CF3D}" name="AocType" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{0CE2507E-1E7F-46FA-9DFF-6AE4A0F8AE3D}" name="Novelty" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{4A4496A0-5A06-4929-A063-D0E1E9A77AEF}" name="Values0" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{F09E181B-A835-4EC7-BA70-8725507DBF0E}" name="Values1" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{2D3EFEBA-8092-4766-9A9E-5C6E2480A95F}" name="Values2" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{B367D252-A7E2-435B-BF61-798C995B65DD}" name="Values3" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{F12D0187-E1B4-4596-A5D9-CD9DD112EC8B}" name="Values4" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{BE84A717-E4C9-4060-801F-90D02748B77B}" name="Values5" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{EA201855-A25A-4BBF-8F12-B90A1F9DA983}" name="Values6" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{1342DCA5-069A-4618-907B-977B7419B267}" name="Values7" dataDxfId="53"/>
+    <tableColumn id="14" xr3:uid="{8BF60613-70C3-4129-9B82-61B27A15DD0A}" name="Values8" dataDxfId="52"/>
+    <tableColumn id="15" xr3:uid="{B678D75B-A8F5-4D48-B43A-89E693998742}" name="Values9" dataDxfId="51"/>
+    <tableColumn id="16" xr3:uid="{D4250E50-1CA8-4235-BFD3-1BD4A07D00A1}" name="Values10" dataDxfId="50"/>
+    <tableColumn id="17" xr3:uid="{C32C3D00-58A9-4F5F-9F77-98A1600B4090}" name="Values11" dataDxfId="49"/>
+    <tableColumn id="18" xr3:uid="{C0F084FF-D73C-42FE-953D-9503B9FBA1D9}" name="Values12" dataDxfId="48"/>
+    <tableColumn id="19" xr3:uid="{4CA9DDF4-75D8-445C-BA30-92C35B3B38BC}" name="Values13" dataDxfId="47"/>
+    <tableColumn id="20" xr3:uid="{91AC5DB7-43C2-43E6-8C77-3CC72659F063}" name="Values14" dataDxfId="46"/>
+    <tableColumn id="21" xr3:uid="{1BBB1A5B-8B5B-486A-891D-B4A1C9082DFE}" name="Values15" dataDxfId="45"/>
+    <tableColumn id="22" xr3:uid="{0D8C5DD0-B37C-4C9D-9266-6044E3A7DB8D}" name="Values16" dataDxfId="44"/>
+    <tableColumn id="23" xr3:uid="{33A81AD7-1832-4C46-AEF2-5C368E05967C}" name="Values17" dataDxfId="43"/>
+    <tableColumn id="24" xr3:uid="{997B6047-2D5A-4E8B-8AA7-704DFD287C6F}" name="Values18" dataDxfId="42"/>
+    <tableColumn id="25" xr3:uid="{4634F739-DE22-4360-AAEB-03AD567C15DA}" name="Values19" dataDxfId="41"/>
+    <tableColumn id="26" xr3:uid="{599822A0-614B-4E5D-80BE-F9043BB08E49}" name="Values20" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{90FE5D9E-D548-45EF-9367-39935624A124}" name="Values21" dataDxfId="39"/>
+    <tableColumn id="27" xr3:uid="{85D5F657-759A-4712-B5DE-720CBCF26E4B}" name="Values22" dataDxfId="38"/>
+    <tableColumn id="28" xr3:uid="{E9721D75-FD9D-4D41-93B8-3835542A4DFD}" name="Values23" dataDxfId="37"/>
+    <tableColumn id="29" xr3:uid="{D1B8B506-E4B7-4569-A829-DDE7BD873338}" name="Values24" dataDxfId="36"/>
+    <tableColumn id="30" xr3:uid="{68DD6566-2B1A-4FCD-9406-10E045AB9FC3}" name="Values25" dataDxfId="35"/>
+    <tableColumn id="31" xr3:uid="{D9715912-18AD-4EE1-A4E7-7DCBB6154841}" name="Values26" dataDxfId="34"/>
+    <tableColumn id="32" xr3:uid="{409EA3C3-CBB6-45BB-9AD9-F27FA2EEE75A}" name="Values27" dataDxfId="33"/>
+    <tableColumn id="33" xr3:uid="{CC13B876-4439-477D-862F-C1CE176ED3EF}" name="Values28" dataDxfId="32"/>
+    <tableColumn id="34" xr3:uid="{C093EFFE-0BE0-425B-95B3-2AD5809464F6}" name="Values29" dataDxfId="31"/>
+    <tableColumn id="35" xr3:uid="{29401921-5C52-483C-AD3C-F679BDFB9693}" name="Values30" dataDxfId="30"/>
+    <tableColumn id="36" xr3:uid="{D7532586-D5C1-4D46-B271-D6CFEA9E6188}" name="Values31" dataDxfId="29"/>
+    <tableColumn id="37" xr3:uid="{966208B7-568C-4CCE-8754-AB8669FAC75B}" name="Values32" dataDxfId="28"/>
+    <tableColumn id="38" xr3:uid="{0281DD50-7612-4D9E-A3DF-2A96F14D1876}" name="Values33" dataDxfId="27"/>
+    <tableColumn id="39" xr3:uid="{AE4AB3E8-BC6A-431F-8D06-F2D47AB85939}" name="Values34" dataDxfId="26"/>
+    <tableColumn id="40" xr3:uid="{15C1375E-B3D5-4C69-B435-EB691FC57530}" name="Values35" dataDxfId="25"/>
+    <tableColumn id="41" xr3:uid="{97CC778D-7683-4D7A-A7B3-2110F1C65233}" name="Values36" dataDxfId="24"/>
+    <tableColumn id="42" xr3:uid="{5FD5F262-95FB-4E9D-BEB3-6C6D84B32413}" name="Values37" dataDxfId="23"/>
+    <tableColumn id="43" xr3:uid="{848095A8-C23E-42A9-B06D-5333C243FA5C}" name="Values38" dataDxfId="22"/>
+    <tableColumn id="44" xr3:uid="{85964CE1-7ED9-4A7C-87CC-B2D8AA20B27C}" name="Values39" dataDxfId="21"/>
+    <tableColumn id="45" xr3:uid="{8616F7A8-146A-400F-973A-321075548F59}" name="Values40" dataDxfId="20"/>
+    <tableColumn id="46" xr3:uid="{98652DE7-A933-4601-8BCD-3661134364D9}" name="Values41" dataDxfId="19"/>
+    <tableColumn id="47" xr3:uid="{FC1105B6-5ADE-4A27-9D20-40A85A2095D8}" name="Values42" dataDxfId="18"/>
+    <tableColumn id="48" xr3:uid="{74BFE3CB-925A-4D76-8EF1-945ED5944C23}" name="Values43" dataDxfId="17"/>
+    <tableColumn id="49" xr3:uid="{D46C6181-8C83-4DF3-B2FF-F4DC0D64FEA7}" name="Values44" dataDxfId="16"/>
+    <tableColumn id="50" xr3:uid="{A225C451-73D9-4EE8-8DBE-366BBDDCB67A}" name="Values45" dataDxfId="15"/>
+    <tableColumn id="51" xr3:uid="{CE7C8271-37F0-4134-B7BA-EF3A6B386467}" name="Values46" dataDxfId="14"/>
+    <tableColumn id="52" xr3:uid="{EA0D7F88-BDDD-4508-A8E5-3D6E6F39CF1A}" name="Values47" dataDxfId="13"/>
+    <tableColumn id="53" xr3:uid="{86A9A3B3-8231-452F-A40C-C0500106CF4E}" name="Values48" dataDxfId="12"/>
+    <tableColumn id="54" xr3:uid="{9DF9D777-0837-43B3-A416-A64EF8ADFFC9}" name="Values49" dataDxfId="11"/>
+    <tableColumn id="55" xr3:uid="{8DFBC52A-3573-4628-B15A-3AF6623963CB}" name="Values50" dataDxfId="10"/>
+    <tableColumn id="56" xr3:uid="{1AE8DABF-E8B7-4171-B162-06FAF8822FA3}" name="Values51" dataDxfId="9"/>
+    <tableColumn id="57" xr3:uid="{E88A0D9B-871A-49A3-90EC-4CFD8E040ED3}" name="Values52" dataDxfId="8"/>
+    <tableColumn id="58" xr3:uid="{AF97704E-6569-449F-AEE2-720AD55CFE27}" name="Values53" dataDxfId="7"/>
+    <tableColumn id="59" xr3:uid="{EF5EF015-6478-469D-B768-B6F779901DEF}" name="Values54" dataDxfId="6"/>
+    <tableColumn id="60" xr3:uid="{D0FFC482-D261-497F-81F5-3A5A89AD0CB4}" name="Values55" dataDxfId="5"/>
+    <tableColumn id="61" xr3:uid="{A91BDB4A-3B29-49D9-9977-CD6E8F2CB52D}" name="Values56" dataDxfId="4"/>
+    <tableColumn id="62" xr3:uid="{CAB70D4D-6ABC-4F86-BB77-4E3D3AC4E49C}" name="Values57" dataDxfId="3"/>
+    <tableColumn id="63" xr3:uid="{05EBBB08-C5AC-44A5-9874-71357C7FAEF3}" name="Values58" dataDxfId="2"/>
+    <tableColumn id="64" xr3:uid="{0AA6597B-36DA-4413-93B3-D374F7F39BB9}" name="Values59" dataDxfId="1"/>
+    <tableColumn id="65" xr3:uid="{7C36714F-66FB-429A-93A5-9EE522E7A2B9}" name="Values60" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1484,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF902ED-C214-4F96-9503-445B7BE7E04C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1535,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59E8FC3-4B20-424B-A44D-77DCF1F6F0A1}">
-  <dimension ref="A1:BV6"/>
+  <dimension ref="A1:BV9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,7 +1559,7 @@
     <col min="16" max="26" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1750,7 +1759,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1767,188 +1776,196 @@
         <v>82</v>
       </c>
       <c r="F2" s="1">
-        <v>-62.400000000000006</v>
+        <v>-80</v>
       </c>
       <c r="G2" s="1">
-        <v>-62.573111721416794</v>
+        <v>-80.079999999999984</v>
       </c>
       <c r="H2" s="1">
-        <v>-62.744207957977196</v>
+        <v>-80.240159999999989</v>
       </c>
       <c r="I2" s="1">
-        <v>-62.967805043069696</v>
+        <v>-80.480880479999982</v>
       </c>
       <c r="J2" s="1">
-        <v>-63.249609137640363</v>
+        <v>-80.802804001919981</v>
       </c>
       <c r="K2" s="1">
-        <v>-63.592360432027142</v>
+        <v>-81.206818021929578</v>
       </c>
       <c r="L2" s="1">
-        <v>-63.998019127576292</v>
+        <v>-81.694058930061161</v>
       </c>
       <c r="M2" s="1">
-        <v>-64.468326832039168</v>
+        <v>-82.265917342571584</v>
       </c>
       <c r="N2" s="1">
-        <v>-65.005016069293589</v>
+        <v>-82.924044681312154</v>
       </c>
       <c r="O2" s="1">
-        <v>-65.60990798276535</v>
+        <v>-83.67036108344395</v>
       </c>
       <c r="P2" s="1">
-        <v>-66.284966318698437</v>
+        <v>-84.507064694278384</v>
       </c>
       <c r="Q2" s="1">
-        <v>-67.116071824382175</v>
+        <v>-85.521149470609728</v>
       </c>
       <c r="R2" s="1">
-        <v>-68.088972842995545</v>
+        <v>-86.718445563198259</v>
       </c>
       <c r="S2" s="1">
-        <v>-69.209864527190149</v>
+        <v>-88.10594069220943</v>
       </c>
       <c r="T2" s="1">
-        <v>-70.485729590990118</v>
+        <v>-89.691847624669194</v>
       </c>
       <c r="U2" s="1">
-        <v>-71.92447079938556</v>
+        <v>-91.485684577162573</v>
       </c>
       <c r="V2" s="1">
-        <v>-73.535024616894404</v>
+        <v>-93.498369637860151</v>
       </c>
       <c r="W2" s="1">
-        <v>-75.327471768758045</v>
+        <v>-95.742330509168795</v>
       </c>
       <c r="X2" s="1">
-        <v>-77.490052125820085</v>
+        <v>-98.423115763425528</v>
       </c>
       <c r="Y2" s="1">
-        <v>-80.021038522117266</v>
+        <v>-101.57265546785514</v>
       </c>
       <c r="Z2" s="1">
-        <v>-82.951717075544892</v>
+        <v>-105.22927106469793</v>
       </c>
       <c r="AA2" s="1">
-        <v>-86.318891036460485</v>
+        <v>-109.43844190728585</v>
       </c>
       <c r="AB2" s="1">
-        <v>-90.165682780609657</v>
+        <v>-114.25373335120644</v>
       </c>
       <c r="AC2" s="1">
-        <v>-94.542461986817372</v>
+        <v>-119.73791255206434</v>
       </c>
       <c r="AD2" s="1">
-        <v>-99.507936187495403</v>
+        <v>-125.9642840047717</v>
       </c>
       <c r="AE2" s="1">
-        <v>-105.13044034380748</v>
+        <v>-133.01828390903893</v>
       </c>
       <c r="AF2" s="1">
-        <v>-111.60718793157646</v>
+        <v>-141.13239922749028</v>
       </c>
       <c r="AG2" s="1">
-        <v>-119.03852890783291</v>
+        <v>-150.44713757650464</v>
       </c>
       <c r="AH2" s="1">
-        <v>-127.55756367665276</v>
+        <v>-161.12888434443647</v>
       </c>
       <c r="AI2" s="1">
-        <v>-137.32184450480466</v>
+        <v>-173.37467955461366</v>
       </c>
       <c r="AJ2" s="1">
-        <v>-148.51803474861973</v>
+        <v>-187.41802859853738</v>
       </c>
       <c r="AK2" s="1">
-        <v>-161.36757961245462</v>
+        <v>-203.53597905801161</v>
       </c>
       <c r="AL2" s="1">
-        <v>-176.13362128347933</v>
+        <v>-222.05775315229064</v>
       </c>
       <c r="AM2" s="1">
-        <v>-193.12944888784196</v>
+        <v>-243.37529745491057</v>
       </c>
       <c r="AN2" s="1">
-        <v>-211.24585051107354</v>
+        <v>-266.2525754156722</v>
       </c>
       <c r="AO2" s="1">
-        <v>-230.4065870862506</v>
+        <v>-290.48155977849837</v>
       </c>
       <c r="AP2" s="1">
-        <v>-250.35940938713679</v>
+        <v>-315.75345547922774</v>
       </c>
       <c r="AQ2" s="1">
-        <v>-271.03667595258645</v>
+        <v>-341.96099228400362</v>
       </c>
       <c r="AR2" s="1">
-        <v>-292.33520596425137</v>
+        <v>-368.97591067443989</v>
       </c>
       <c r="AS2" s="1">
-        <v>-313.81139412494559</v>
+        <v>-396.28012806434845</v>
       </c>
       <c r="AT2" s="1">
-        <v>-335.29119824983485</v>
+        <v>-423.62345690078848</v>
       </c>
       <c r="AU2" s="1">
-        <v>-356.5587629078824</v>
+        <v>-450.735358142439</v>
       </c>
       <c r="AV2" s="1">
-        <v>-376.98585400563792</v>
+        <v>-476.8780089147005</v>
       </c>
       <c r="AW2" s="1">
-        <v>-396.30844958709582</v>
+        <v>-501.67566537826497</v>
       </c>
       <c r="AX2" s="1">
-        <v>-413.32760330752188</v>
+        <v>-523.74939465490866</v>
       </c>
       <c r="AY2" s="1">
-        <v>-427.25659795511325</v>
+        <v>-542.08062346783038</v>
       </c>
       <c r="AZ2" s="1">
-        <v>-436.73021271730363</v>
+        <v>-555.0905584310583</v>
       </c>
       <c r="BA2" s="1">
-        <v>-440.85660676388068</v>
+        <v>-561.75164513223103</v>
       </c>
       <c r="BB2" s="1">
-        <v>-440.82997931846097</v>
+        <v>-563.43690006762768</v>
       </c>
       <c r="BC2" s="1">
-        <v>-438.74050211348998</v>
+        <v>-560.05627866722193</v>
       </c>
       <c r="BD2" s="1">
-        <v>-430.06181630174956</v>
+        <v>-546.61492797920857</v>
       </c>
       <c r="BE2" s="1">
-        <v>-403.95406817909753</v>
+        <v>-510.53834273258076</v>
       </c>
       <c r="BF2" s="1">
-        <v>-367.73088041921051</v>
+        <v>-463.56881520118333</v>
       </c>
       <c r="BG2" s="1">
-        <v>-323.68571140370199</v>
+        <v>-407.01341974663899</v>
       </c>
       <c r="BH2" s="1">
-        <v>-273.57128742844264</v>
+        <v>-343.11231284641667</v>
       </c>
       <c r="BI2" s="1">
-        <v>-220.25128050271982</v>
+        <v>-275.51918721567256</v>
       </c>
       <c r="BJ2" s="1">
-        <v>-166.33124150811673</v>
+        <v>-207.46594797340143</v>
       </c>
       <c r="BK2" s="1">
-        <v>-115.62636533208395</v>
+        <v>-143.77390194556719</v>
       </c>
       <c r="BL2" s="1">
-        <v>-72.269898774664426</v>
+        <v>-89.571140912088353</v>
       </c>
       <c r="BM2" s="1">
-        <v>-37.740842268239504</v>
+        <v>-46.576993274285947</v>
       </c>
       <c r="BN2" s="1">
-        <v>-11.410122760645162</v>
-      </c>
+        <v>-13.973097982285781</v>
+      </c>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1"/>
+      <c r="BQ2" s="1"/>
+      <c r="BR2" s="1"/>
+      <c r="BS2" s="1"/>
+      <c r="BT2" s="1"/>
+      <c r="BU2" s="1"/>
+      <c r="BV2" s="1"/>
     </row>
     <row r="3" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1961,193 +1978,193 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="F3" s="1">
-        <v>-76</v>
+        <v>-73.600000000000009</v>
       </c>
       <c r="G3" s="1">
-        <v>-76.210841199161464</v>
+        <v>-73.804183056030055</v>
       </c>
       <c r="H3" s="1">
-        <v>-76.419227641126056</v>
+        <v>-74.005988873511555</v>
       </c>
       <c r="I3" s="1">
-        <v>-76.691557424251542</v>
+        <v>-74.269718768748874</v>
       </c>
       <c r="J3" s="1">
-        <v>-77.034780359946595</v>
+        <v>-74.602103085421973</v>
       </c>
       <c r="K3" s="1">
-        <v>-77.452233859520234</v>
+        <v>-75.006373842903812</v>
       </c>
       <c r="L3" s="1">
-        <v>-77.946305347689076</v>
+        <v>-75.484843073551531</v>
       </c>
       <c r="M3" s="1">
-        <v>-78.519116013381037</v>
+        <v>-76.039564981379542</v>
       </c>
       <c r="N3" s="1">
-        <v>-79.172775981831933</v>
+        <v>-76.672583056089877</v>
       </c>
       <c r="O3" s="1">
-        <v>-79.909503312342409</v>
+        <v>-77.386045313005297</v>
       </c>
       <c r="P3" s="1">
-        <v>-80.731689747132705</v>
+        <v>-78.182267965644314</v>
       </c>
       <c r="Q3" s="1">
-        <v>-81.743933632260322</v>
+        <v>-79.162546254399487</v>
       </c>
       <c r="R3" s="1">
-        <v>-82.92887718057149</v>
+        <v>-80.310070532763987</v>
       </c>
       <c r="S3" s="1">
-        <v>-84.294065770295688</v>
+        <v>-81.632147903865302</v>
       </c>
       <c r="T3" s="1">
-        <v>-85.848003989026424</v>
+        <v>-83.137014389372965</v>
       </c>
       <c r="U3" s="1">
-        <v>-87.600316999251646</v>
+        <v>-84.833991199275289</v>
       </c>
       <c r="V3" s="1">
-        <v>-89.56188895647395</v>
+        <v>-86.733618778901089</v>
       </c>
       <c r="W3" s="1">
-        <v>-91.744997667077087</v>
+        <v>-88.847787214432557</v>
       </c>
       <c r="X3" s="1">
-        <v>-94.378909640421881</v>
+        <v>-91.398523020198041</v>
       </c>
       <c r="Y3" s="1">
-        <v>-97.461521276937688</v>
+        <v>-94.38378902608703</v>
       </c>
       <c r="Z3" s="1">
-        <v>-101.03093746380466</v>
+        <v>-97.84048680705294</v>
       </c>
       <c r="AA3" s="1">
-        <v>-105.13198267261211</v>
+        <v>-101.81202532505596</v>
       </c>
       <c r="AB3" s="1">
-        <v>-109.81717774561433</v>
+        <v>-106.34926686943705</v>
       </c>
       <c r="AC3" s="1">
-        <v>-115.14787036855961</v>
+        <v>-111.51162183060511</v>
       </c>
       <c r="AD3" s="1">
-        <v>-121.19556330528285</v>
+        <v>-117.36833499037918</v>
       </c>
       <c r="AE3" s="1">
-        <v>-128.04348503412447</v>
+        <v>-124.00000655936267</v>
       </c>
       <c r="AF3" s="1">
-        <v>-135.93183145512518</v>
+        <v>-131.63924730391071</v>
       </c>
       <c r="AG3" s="1">
-        <v>-144.98282366979649</v>
+        <v>-140.40441871180292</v>
       </c>
       <c r="AH3" s="1">
-        <v>-155.35857114464116</v>
+        <v>-150.45251100323148</v>
       </c>
       <c r="AI3" s="1">
-        <v>-167.25096446098001</v>
+        <v>-161.96935505694907</v>
       </c>
       <c r="AJ3" s="1">
-        <v>-180.88735001434452</v>
+        <v>-175.17511790862838</v>
       </c>
       <c r="AK3" s="1">
-        <v>-196.53743670747676</v>
+        <v>-190.33099133776699</v>
       </c>
       <c r="AL3" s="1">
-        <v>-214.52171822987864</v>
+        <v>-207.74734818051408</v>
       </c>
       <c r="AM3" s="1">
-        <v>-235.22176467108955</v>
+        <v>-227.79370894463409</v>
       </c>
       <c r="AN3" s="1">
-        <v>-257.28661280194854</v>
+        <v>-249.16177239767649</v>
       </c>
       <c r="AO3" s="1">
-        <v>-280.62340734863852</v>
+        <v>-271.76161553762893</v>
       </c>
       <c r="AP3" s="1">
-        <v>-304.92492168946148</v>
+        <v>-295.29571363611007</v>
       </c>
       <c r="AQ3" s="1">
-        <v>-330.10877199353479</v>
+        <v>-319.68428445689688</v>
       </c>
       <c r="AR3" s="1">
-        <v>-356.04928931543435</v>
+        <v>-344.80562754757858</v>
       </c>
       <c r="AS3" s="1">
-        <v>-382.20618515217734</v>
+        <v>-370.13651614737176</v>
       </c>
       <c r="AT3" s="1">
-        <v>-408.36748504787579</v>
+        <v>-395.47166973057449</v>
       </c>
       <c r="AU3" s="1">
-        <v>-434.27028815703625</v>
+        <v>-420.55648958365617</v>
       </c>
       <c r="AV3" s="1">
-        <v>-459.14943757096921</v>
+        <v>-444.64998164767547</v>
       </c>
       <c r="AW3" s="1">
-        <v>-482.68336808684745</v>
+        <v>-467.44073541042076</v>
       </c>
       <c r="AX3" s="1">
-        <v>-503.41182454121252</v>
+        <v>-487.51460902938481</v>
       </c>
       <c r="AY3" s="1">
-        <v>-520.37662571456099</v>
+        <v>-503.94367963936435</v>
       </c>
       <c r="AZ3" s="1">
-        <v>-531.91500266851074</v>
+        <v>-515.11768679476836</v>
       </c>
       <c r="BA3" s="1">
-        <v>-536.94073900729052</v>
+        <v>-519.98471567021829</v>
       </c>
       <c r="BB3" s="1">
-        <v>-536.90830814427932</v>
+        <v>-519.95330893972323</v>
       </c>
       <c r="BC3" s="1">
-        <v>-534.36343206130186</v>
+        <v>-517.48879736462914</v>
       </c>
       <c r="BD3" s="1">
-        <v>-523.79323780341292</v>
+        <v>-507.25239871488412</v>
       </c>
       <c r="BE3" s="1">
-        <v>-491.99533944890078</v>
+        <v>-476.45864451893556</v>
       </c>
       <c r="BF3" s="1">
-        <v>-447.87735435673068</v>
+        <v>-433.73385895599188</v>
       </c>
       <c r="BG3" s="1">
-        <v>-394.23259722245751</v>
+        <v>-381.78314678385362</v>
       </c>
       <c r="BH3" s="1">
-        <v>-333.19579879105191</v>
+        <v>-322.67382619765033</v>
       </c>
       <c r="BI3" s="1">
-        <v>-268.25476471485104</v>
+        <v>-259.78356161859261</v>
       </c>
       <c r="BJ3" s="1">
-        <v>-202.58292234962934</v>
+        <v>-196.18556690700947</v>
       </c>
       <c r="BK3" s="1">
-        <v>-140.82698341728172</v>
+        <v>-136.3798155198939</v>
       </c>
       <c r="BL3" s="1">
-        <v>-88.021030558886153</v>
+        <v>-85.241419067552911</v>
       </c>
       <c r="BM3" s="1">
-        <v>-45.966410454907084</v>
+        <v>-44.514839598436339</v>
       </c>
       <c r="BN3" s="1">
-        <v>-13.896944387965261</v>
+        <v>-13.458093512555834</v>
       </c>
       <c r="BO3" s="1"/>
       <c r="BP3" s="1"/>
@@ -2163,199 +2180,199 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="F4" s="1">
-        <v>2100.0225</v>
+        <v>-80</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>-80.221938104380499</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>-80.441292253816911</v>
       </c>
       <c r="I4" s="1">
-        <v>1839.2492126649859</v>
+        <v>-80.727955183422679</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>-81.089242484154312</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>-81.528667220547618</v>
       </c>
       <c r="L4" s="1">
-        <v>1635.3731331102413</v>
+        <v>-82.048742471251657</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>-82.651701066716882</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>-83.33976419140204</v>
       </c>
       <c r="O4" s="1">
-        <v>1459.915196900572</v>
+        <v>-84.115266644570966</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>-84.980726049613381</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>-86.046245928695086</v>
       </c>
       <c r="R4" s="1">
-        <v>1305.8106677164712</v>
+        <v>-87.293554926917366</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
+        <v>-88.73059554767967</v>
       </c>
       <c r="T4" s="1">
-        <v>0</v>
+        <v>-90.366319988448865</v>
       </c>
       <c r="U4" s="1">
-        <v>1169.3289851977881</v>
+        <v>-92.210859999212261</v>
       </c>
       <c r="V4" s="1">
-        <v>0</v>
+        <v>-94.275672585762052</v>
       </c>
       <c r="W4" s="1">
-        <v>0</v>
+        <v>-96.573681754817997</v>
       </c>
       <c r="X4" s="1">
-        <v>1047.9266963085413</v>
+        <v>-99.346220674128304</v>
       </c>
       <c r="Y4" s="1">
-        <v>0</v>
+        <v>-102.59107502835546</v>
       </c>
       <c r="Z4" s="1">
-        <v>0</v>
+        <v>-106.34835522505755</v>
       </c>
       <c r="AA4" s="1">
-        <v>939.75325095344851</v>
+        <v>-110.66524491853907</v>
       </c>
       <c r="AB4" s="1">
-        <v>0</v>
+        <v>-115.59702920590982</v>
       </c>
       <c r="AC4" s="1">
-        <v>0</v>
+        <v>-121.2082845984838</v>
       </c>
       <c r="AD4" s="1">
-        <v>843.32397578516316</v>
+        <v>-127.57427716345563</v>
       </c>
       <c r="AE4" s="1">
-        <v>0</v>
+        <v>-134.7826158253942</v>
       </c>
       <c r="AF4" s="1">
-        <v>0</v>
+        <v>-143.08613837381597</v>
       </c>
       <c r="AG4" s="1">
-        <v>757.12221622080835</v>
+        <v>-152.61349859978577</v>
       </c>
       <c r="AH4" s="1">
-        <v>0</v>
+        <v>-163.53533804699072</v>
       </c>
       <c r="AI4" s="1">
-        <v>0</v>
+        <v>-176.05364680103159</v>
       </c>
       <c r="AJ4" s="1">
-        <v>679.97252358402523</v>
+        <v>-190.40773685720475</v>
       </c>
       <c r="AK4" s="1">
-        <v>0</v>
+        <v>-206.88151232365976</v>
       </c>
       <c r="AL4" s="1">
-        <v>0</v>
+        <v>-225.81233497881965</v>
       </c>
       <c r="AM4" s="1">
-        <v>611.00482842712802</v>
+        <v>-247.60185754851531</v>
       </c>
       <c r="AN4" s="1">
-        <v>0</v>
+        <v>-270.8280134757353</v>
       </c>
       <c r="AO4" s="1">
-        <v>0</v>
+        <v>-295.39306036698792</v>
       </c>
       <c r="AP4" s="1">
-        <v>549.23864592775681</v>
+        <v>-320.9736017783805</v>
       </c>
       <c r="AQ4" s="1">
-        <v>0</v>
+        <v>-347.48291788793136</v>
       </c>
       <c r="AR4" s="1">
-        <v>0</v>
+        <v>-374.78872559519408</v>
       </c>
       <c r="AS4" s="1">
-        <v>488.49969417144968</v>
+        <v>-402.32230016018667</v>
       </c>
       <c r="AT4" s="1">
-        <v>0</v>
+        <v>-429.86051057671136</v>
       </c>
       <c r="AU4" s="1">
-        <v>0</v>
+        <v>-457.12661911266974</v>
       </c>
       <c r="AV4" s="1">
-        <v>425.1499177671455</v>
+        <v>-483.3151974431255</v>
       </c>
       <c r="AW4" s="1">
-        <v>0</v>
+        <v>-508.08775588089208</v>
       </c>
       <c r="AX4" s="1">
-        <v>0</v>
+        <v>-529.90718372759216</v>
       </c>
       <c r="AY4" s="1">
-        <v>358.55879861766698</v>
+        <v>-547.76486917322211</v>
       </c>
       <c r="AZ4" s="1">
-        <v>0</v>
+        <v>-559.91052912474822</v>
       </c>
       <c r="BA4" s="1">
-        <v>0</v>
+        <v>-565.20077790241112</v>
       </c>
       <c r="BB4" s="1">
-        <v>295.58606003389389</v>
+        <v>-565.16664015187303</v>
       </c>
       <c r="BC4" s="1">
-        <v>0</v>
+        <v>-562.487823222423</v>
       </c>
       <c r="BD4" s="1">
-        <v>0</v>
+        <v>-551.36130295096098</v>
       </c>
       <c r="BE4" s="1">
-        <v>210.66644204643885</v>
+        <v>-517.88983099884297</v>
       </c>
       <c r="BF4" s="1">
-        <v>0</v>
+        <v>-471.44984669129548</v>
       </c>
       <c r="BG4" s="1">
-        <v>0</v>
+        <v>-414.98168128679742</v>
       </c>
       <c r="BH4" s="1">
-        <v>141.68792271478148</v>
+        <v>-350.73241978005467</v>
       </c>
       <c r="BI4" s="1">
-        <v>0</v>
+        <v>-282.37343654194848</v>
       </c>
       <c r="BJ4" s="1">
-        <v>0</v>
+        <v>-213.24518142066248</v>
       </c>
       <c r="BK4" s="1">
-        <v>85.966932176770044</v>
+        <v>-148.23892991292814</v>
       </c>
       <c r="BL4" s="1">
-        <v>0</v>
+        <v>-92.653716377774899</v>
       </c>
       <c r="BM4" s="1">
-        <v>0</v>
+        <v>-48.385695215691669</v>
       </c>
       <c r="BN4" s="1">
-        <v>45.101293567782378</v>
+        <v>-14.628362513647645</v>
       </c>
       <c r="BO4" s="1"/>
       <c r="BP4" s="1"/>
@@ -2366,30 +2383,1064 @@
       <c r="BU4" s="1"/>
       <c r="BV4" s="1"/>
     </row>
+    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-80</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-80.221938104380499</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-80.441292253816911</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-80.727955183422679</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-81.089242484154312</v>
+      </c>
+      <c r="K5" s="1">
+        <v>-81.528667220547618</v>
+      </c>
+      <c r="L5" s="1">
+        <v>-82.048742471251657</v>
+      </c>
+      <c r="M5" s="1">
+        <v>-82.651701066716882</v>
+      </c>
+      <c r="N5" s="1">
+        <v>-83.33976419140204</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-84.115266644570966</v>
+      </c>
+      <c r="P5" s="1">
+        <v>-84.980726049613381</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>-86.046245928695086</v>
+      </c>
+      <c r="R5" s="1">
+        <v>-87.293554926917366</v>
+      </c>
+      <c r="S5" s="1">
+        <v>-88.73059554767967</v>
+      </c>
+      <c r="T5" s="1">
+        <v>-90.366319988448865</v>
+      </c>
+      <c r="U5" s="1">
+        <v>-92.210859999212261</v>
+      </c>
+      <c r="V5" s="1">
+        <v>-94.275672585762052</v>
+      </c>
+      <c r="W5" s="1">
+        <v>-96.573681754817997</v>
+      </c>
+      <c r="X5" s="1">
+        <v>-99.346220674128304</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>-102.59107502835546</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>-106.34835522505755</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>-110.66524491853907</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>-115.59702920590982</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>-121.2082845984838</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>-127.57427716345563</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>-134.7826158253942</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>-143.08613837381597</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>-152.61349859978577</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>-163.53533804699072</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>-176.05364680103159</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>-190.40773685720475</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>-206.88151232365976</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>-225.81233497881965</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>-247.60185754851531</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>-270.8280134757353</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>-295.39306036698792</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>-320.9736017783805</v>
+      </c>
+      <c r="AQ5" s="1">
+        <v>-347.48291788793136</v>
+      </c>
+      <c r="AR5" s="1">
+        <v>-374.78872559519408</v>
+      </c>
+      <c r="AS5" s="1">
+        <v>-402.32230016018667</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>-429.86051057671136</v>
+      </c>
+      <c r="AU5" s="1">
+        <v>-457.12661911266974</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>-483.3151974431255</v>
+      </c>
+      <c r="AW5" s="1">
+        <v>-508.08775588089208</v>
+      </c>
+      <c r="AX5" s="1">
+        <v>-529.90718372759216</v>
+      </c>
+      <c r="AY5" s="1">
+        <v>-547.76486917322211</v>
+      </c>
+      <c r="AZ5" s="1">
+        <v>-559.91052912474822</v>
+      </c>
+      <c r="BA5" s="1">
+        <v>-565.20077790241112</v>
+      </c>
+      <c r="BB5" s="1">
+        <v>-565.16664015187303</v>
+      </c>
+      <c r="BC5" s="1">
+        <v>-562.487823222423</v>
+      </c>
+      <c r="BD5" s="1">
+        <v>-551.36130295096098</v>
+      </c>
+      <c r="BE5" s="1">
+        <v>-517.88983099884297</v>
+      </c>
+      <c r="BF5" s="1">
+        <v>-471.44984669129548</v>
+      </c>
+      <c r="BG5" s="1">
+        <v>-414.98168128679742</v>
+      </c>
+      <c r="BH5" s="1">
+        <v>-350.73241978005467</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>-282.37343654194848</v>
+      </c>
+      <c r="BJ5" s="1">
+        <v>-213.24518142066248</v>
+      </c>
+      <c r="BK5" s="1">
+        <v>-148.23892991292814</v>
+      </c>
+      <c r="BL5" s="1">
+        <v>-92.653716377774899</v>
+      </c>
+      <c r="BM5" s="1">
+        <v>-48.385695215691669</v>
+      </c>
+      <c r="BN5" s="1">
+        <v>-14.628362513647645</v>
+      </c>
+      <c r="BO5" s="1"/>
+      <c r="BP5" s="1"/>
+      <c r="BQ5" s="1"/>
+      <c r="BR5" s="1"/>
+      <c r="BS5" s="1"/>
+      <c r="BT5" s="1"/>
+      <c r="BU5" s="1"/>
+      <c r="BV5" s="1"/>
+    </row>
     <row r="6" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="F6" s="1"/>
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2210.5500000000002</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1989.4950000000001</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1790.5455000000002</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1611.4909500000001</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1450.3418550000001</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1305.3076695000002</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1174.7769025500002</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>1057.2992122950002</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>951.56929106550024</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>856.41236195895021</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>770.77112576305524</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>693.69401318674977</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>624.32461186807484</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="1">
+        <v>555.64890456258661</v>
+      </c>
+      <c r="AT6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="1">
+        <v>483.41454696945033</v>
+      </c>
+      <c r="AW6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="1">
+        <v>406.06821945433825</v>
+      </c>
+      <c r="AZ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="1">
+        <v>324.85457556347063</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="1">
+        <v>243.64093167260296</v>
+      </c>
+      <c r="BF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="1">
+        <v>168.11224285409602</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="1">
+        <v>104.22959056953954</v>
+      </c>
+      <c r="BL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="1">
+        <v>56.283978907551358</v>
+      </c>
+      <c r="BO6" s="1"/>
+      <c r="BP6" s="1"/>
+      <c r="BQ6" s="1"/>
+      <c r="BR6" s="1"/>
+      <c r="BS6" s="1"/>
+      <c r="BT6" s="1"/>
+      <c r="BU6" s="1"/>
+      <c r="BV6" s="1"/>
+    </row>
+    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2210.5500000000002</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2063.2215160144488</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1882.8080036188367</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1709.2914496442083</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1548.107757870913</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1400.2266747581864</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1265.3600787277182</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>1142.6680434267498</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>1031.1590303291489</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>930.12425790876898</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>838.69960468102829</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>755.89487156573273</v>
+      </c>
+      <c r="AN7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="1">
+        <v>681.03269727904706</v>
+      </c>
+      <c r="AQ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="1">
+        <v>606.47057787820472</v>
+      </c>
+      <c r="AT7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="1">
+        <v>527.46046281648682</v>
+      </c>
+      <c r="AW7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="1">
+        <v>441.49550282763306</v>
+      </c>
+      <c r="AZ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="1">
+        <v>342.98899321869982</v>
+      </c>
+      <c r="BC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="1">
+        <v>269.66796579728577</v>
+      </c>
+      <c r="BF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="1">
+        <v>189.73508154216125</v>
+      </c>
+      <c r="BI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="1">
+        <v>119.40335697364351</v>
+      </c>
+      <c r="BL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="1">
+        <v>65.653826382205708</v>
+      </c>
+      <c r="BO7" s="1"/>
+      <c r="BP7" s="1"/>
+      <c r="BQ7" s="1"/>
+      <c r="BR7" s="1"/>
+      <c r="BS7" s="1"/>
+      <c r="BT7" s="1"/>
+      <c r="BU7" s="1"/>
+      <c r="BV7" s="1"/>
+    </row>
+    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2210.5500000000002</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1936.0518028052484</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1721.4454032739382</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1536.7528388427074</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>1374.5375449647067</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1230.8726159976718</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>1103.0807329563593</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>989.21394837205116</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>887.70944819490865</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>796.97075391664043</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>715.76055114107919</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="1">
+        <v>643.16297729171379</v>
+      </c>
+      <c r="AN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="1">
+        <v>578.14594308184928</v>
+      </c>
+      <c r="AQ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="1">
+        <v>514.21020439099971</v>
+      </c>
+      <c r="AT8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="1">
+        <v>447.52622922857421</v>
+      </c>
+      <c r="AW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="1">
+        <v>377.43031433438631</v>
+      </c>
+      <c r="AZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="1">
+        <v>311.14322108830936</v>
+      </c>
+      <c r="BC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="1">
+        <v>221.75414952256722</v>
+      </c>
+      <c r="BF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="1">
+        <v>149.14518180503313</v>
+      </c>
+      <c r="BI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="1">
+        <v>90.491507554494788</v>
+      </c>
+      <c r="BL8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="1">
+        <v>47.475045860823556</v>
+      </c>
+      <c r="BO8" s="1"/>
+      <c r="BP8" s="1"/>
+      <c r="BQ8" s="1"/>
+      <c r="BR8" s="1"/>
+      <c r="BS8" s="1"/>
+      <c r="BT8" s="1"/>
+      <c r="BU8" s="1"/>
+      <c r="BV8" s="1"/>
+    </row>
+    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2210.5500000000002</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1936.0518028052484</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1721.4454032739382</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1536.7528388427074</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1374.5375449647067</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1230.8726159976718</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>1103.0807329563593</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>989.21394837205116</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>887.70944819490865</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>796.97075391664043</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>715.76055114107919</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="1">
+        <v>643.16297729171379</v>
+      </c>
+      <c r="AN9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="1">
+        <v>578.14594308184928</v>
+      </c>
+      <c r="AQ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="1">
+        <v>514.21020439099971</v>
+      </c>
+      <c r="AT9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="1">
+        <v>447.52622922857421</v>
+      </c>
+      <c r="AW9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="1">
+        <v>377.43031433438631</v>
+      </c>
+      <c r="AZ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="1">
+        <v>311.14322108830936</v>
+      </c>
+      <c r="BC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="1">
+        <v>221.75414952256722</v>
+      </c>
+      <c r="BF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="1">
+        <v>149.14518180503313</v>
+      </c>
+      <c r="BI9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="1">
+        <v>90.491507554494788</v>
+      </c>
+      <c r="BL9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN9" s="1">
+        <v>47.475045860823556</v>
+      </c>
+      <c r="BO9" s="1"/>
+      <c r="BP9" s="1"/>
+      <c r="BQ9" s="1"/>
+      <c r="BR9" s="1"/>
+      <c r="BS9" s="1"/>
+      <c r="BT9" s="1"/>
+      <c r="BU9" s="1"/>
+      <c r="BV9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="A2:A4" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>GroupOfContract_SystemName</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="E2:E9" xr:uid="{0F7E7F28-792F-463C-A61C-1C46296B9633}">
+      <formula1>Novelty_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D9" xr:uid="{6B4B47A9-C9B6-46FD-AC51-39AF8A737A35}">
+      <formula1>VariableType_SystemName</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="B2:C9" xr:uid="{C1473488-71A4-45AD-A7F0-BE10261E97AB}">
       <formula1>AmountType_SystemName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-0100-000002000000}">
-      <formula1>VariableType_SystemName</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E4" xr:uid="{00000000-0002-0000-0100-000004000000}">
-      <formula1>Novelty_SystemName</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="A2:A9" xr:uid="{68F8460D-C0F8-4BA9-B047-C7A65AED9257}">
+      <formula1>GroupOfContract_SystemName</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="D1 E1 B1" numberStoredAsText="1" calculatedColumn="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>